<commit_message>
config.yaml now modified for new design of workflow; grid.tsv renamed to samples.tsv
</commit_message>
<xml_diff>
--- a/config/stock_matrix/test_subset_Mu-seq_8_Stock_matrix.xlsx
+++ b/config/stock_matrix/test_subset_Mu-seq_8_Stock_matrix.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t xml:space="preserve">Col_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Col_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Col_03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Col_04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Row_01</t>
+    <t xml:space="preserve">Col-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Row-01</t>
   </si>
   <si>
     <t xml:space="preserve">D-0078</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">D-0081</t>
   </si>
   <si>
-    <t xml:space="preserve">Row_02</t>
+    <t xml:space="preserve">Row-02</t>
   </si>
   <si>
     <t xml:space="preserve">D-0102</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">D-0105</t>
   </si>
   <si>
-    <t xml:space="preserve">Row_03</t>
+    <t xml:space="preserve">Row-03</t>
   </si>
   <si>
     <t xml:space="preserve">D-0126</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">D-0129</t>
   </si>
   <si>
-    <t xml:space="preserve">Row_04</t>
+    <t xml:space="preserve">Row-04</t>
   </si>
   <si>
     <t xml:space="preserve">D-0150</t>
@@ -350,10 +350,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>

</xml_diff>

<commit_message>
updated to use underscore like our actual stock matrix tables
</commit_message>
<xml_diff>
--- a/config/stock_matrix/test_subset_Mu-seq_8_Stock_matrix.xlsx
+++ b/config/stock_matrix/test_subset_Mu-seq_8_Stock_matrix.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t xml:space="preserve">Col-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Col-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Col-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Col-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Row-01</t>
+    <t xml:space="preserve">Col_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Row_01</t>
   </si>
   <si>
     <t xml:space="preserve">D-0078</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">D-0081</t>
   </si>
   <si>
-    <t xml:space="preserve">Row-02</t>
+    <t xml:space="preserve">Row_02</t>
   </si>
   <si>
     <t xml:space="preserve">D-0102</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">D-0105</t>
   </si>
   <si>
-    <t xml:space="preserve">Row-03</t>
+    <t xml:space="preserve">Row_03</t>
   </si>
   <si>
     <t xml:space="preserve">D-0126</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">D-0129</t>
   </si>
   <si>
-    <t xml:space="preserve">Row-04</t>
+    <t xml:space="preserve">Row_04</t>
   </si>
   <si>
     <t xml:space="preserve">D-0150</t>
@@ -350,10 +350,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>

</xml_diff>